<commit_message>
Almost ready for delivering
</commit_message>
<xml_diff>
--- a/Useful data_files/OCL3/beam.xlsx
+++ b/Useful data_files/OCL3/beam.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="4935" yWindow="9000" windowWidth="19980" windowHeight="16440" tabRatio="500" firstSheet="4" activeTab="6"/>
+    <workbookView xWindow="4935" yWindow="9000" windowWidth="19980" windowHeight="16440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Beam profile 14-15 nov" sheetId="1" r:id="rId1"/>
@@ -2126,8 +2126,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:X43"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2853,6 +2853,9 @@
       <c r="B14">
         <v>-2</v>
       </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
       <c r="D14">
         <v>158</v>
       </c>
@@ -2910,6 +2913,9 @@
     <row r="15" spans="1:24">
       <c r="B15">
         <v>-2.5</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
       </c>
       <c r="D15">
         <v>104</v>
@@ -11192,7 +11198,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:AA35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K5" sqref="K5:K8"/>
     </sheetView>
   </sheetViews>

</xml_diff>